<commit_message>
Fixed AA position cut site bug
AA position cut site bug fixed. Visualization updates to final figure
</commit_message>
<xml_diff>
--- a/Data/20241217_BARD1_sgRNA_cutsites.xlsx
+++ b/Data/20241217_BARD1_sgRNA_cutsites.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10511"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10720"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ivan/Documents/GitHub/BARD1_SGE_analysis/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C97D2C5C-8841-4843-B792-3902C68BA19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1E38734-6D38-734D-A18C-E7FB18F3E261}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16080" xr2:uid="{F7E8E1AA-ADEC-1649-9091-979EB602F4D1}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{F7E8E1AA-ADEC-1649-9091-979EB602F4D1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>target</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>BARD1_X4I</t>
+  </si>
+  <si>
+    <t>AApos</t>
   </si>
 </sst>
 </file>
@@ -529,10 +532,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EA78282-5204-2942-8B1A-6BC9A66E1CB7}">
-  <dimension ref="A1:B35"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="F28" sqref="F28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -541,284 +544,389 @@
     <col min="2" max="2" width="11.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="1">
         <v>214809491</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>214809491</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="1">
         <v>214797066</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="1">
         <v>214792399</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>4</v>
       </c>
       <c r="B6" s="1">
         <v>214792363</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>214781493</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>214781425</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>9</v>
       </c>
       <c r="B9" s="1">
         <v>214781318</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" s="2">
         <v>214781298</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" s="2">
         <v>214781162</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>12</v>
       </c>
       <c r="B12" s="2">
         <v>214781033</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>13</v>
       </c>
       <c r="B13" s="2">
         <v>214780998</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>14</v>
       </c>
       <c r="B14" s="1">
         <v>214780883</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>35</v>
       </c>
       <c r="B15" s="2">
         <v>214780856</v>
       </c>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>214780718</v>
       </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C16">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
       <c r="B17" s="1">
         <v>214780665</v>
       </c>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C17">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>17</v>
       </c>
       <c r="B18" s="2">
         <v>214780619</v>
       </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C18">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>18</v>
       </c>
       <c r="B19" s="2">
         <v>214769298</v>
       </c>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C19">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>19</v>
       </c>
       <c r="B20" s="2">
         <v>214769247</v>
       </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>20</v>
       </c>
       <c r="B21" s="2">
         <v>214767624</v>
       </c>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>21</v>
       </c>
       <c r="B22" s="2">
         <v>214767540</v>
       </c>
-    </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>504</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>22</v>
       </c>
       <c r="B23" s="2">
         <v>214767501</v>
       </c>
-    </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>517</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>23</v>
       </c>
       <c r="B24" s="2">
         <v>214752531</v>
       </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C24">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>24</v>
       </c>
       <c r="B25" s="2">
         <v>214752464</v>
       </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C25">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>25</v>
       </c>
       <c r="B26" s="2">
         <v>214745810</v>
       </c>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C26">
+        <v>575</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>34</v>
       </c>
       <c r="B27" s="2">
         <v>214745758</v>
       </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C27">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>26</v>
       </c>
       <c r="B28" s="2">
         <v>214745137</v>
       </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C28">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>27</v>
       </c>
       <c r="B29" s="2">
         <v>214745115</v>
       </c>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C29">
+        <v>619</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>28</v>
       </c>
       <c r="B30" s="2">
         <v>214730451</v>
       </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C30">
+        <v>654</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>29</v>
       </c>
       <c r="B31" s="2">
         <v>214730435</v>
       </c>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C31">
+        <v>659</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>30</v>
       </c>
       <c r="B32" s="2">
         <v>214728960</v>
       </c>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C32">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>31</v>
       </c>
       <c r="B33" s="2">
         <v>214728858</v>
       </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C33">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>32</v>
       </c>
       <c r="B34" s="2">
         <v>214728828</v>
       </c>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C34">
+        <v>728</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>33</v>
       </c>
       <c r="B35" s="2">
         <v>214728699</v>
+      </c>
+      <c r="C35">
+        <v>771</v>
       </c>
     </row>
   </sheetData>

</xml_diff>